<commit_message>
Se agrega SDatoTipo, modificaciones de SProyectoPropiedad, se agrega el component peppropiedad
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -2087,7 +2087,7 @@
   <dimension ref="A1:E99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,7 +2380,7 @@
         <v>221</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3576,7 +3576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
@@ -4791,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5173,7 +5173,7 @@
         <v>449</v>
       </c>
       <c r="C34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -5739,7 +5739,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -5764,7 +5764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
@@ -6935,7 +6935,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.19565217391304349</v>
+        <v>0.20652173913043478</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>7.8260869565217392</v>
+        <v>8.2608695652173907</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>55.957690292944349</v>
+        <v>56.392472901640005</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.26148453407917921</v>
+        <v>0.26351622851233647</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados en la aplicación
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -1524,7 +1524,7 @@
     <t>prestamotipo</t>
   </si>
   <si>
-    <t>peotipo</t>
+    <t>peptipo</t>
   </si>
 </sst>
 </file>
@@ -4791,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5184,7 +5184,7 @@
         <v>498</v>
       </c>
       <c r="C35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -5739,7 +5739,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -6934,8 +6934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>6.05</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>7.2891566265060243E-2</v>
+        <v>9.6987951807228925E-2</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>8.7469879518072293</v>
+        <v>11.638554216867471</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>56.392472901640005</v>
+        <v>59.284039166700246</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.26351622851233647</v>
+        <v>0.27702822040514136</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Se agrega controlador de Colaborador, se realizan cambios en Entidades, se agregan nuevos modales y se modifican los existentes.
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2290,7 @@
         <v>215</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,7 +3672,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.20652173913043478</v>
+        <v>0.21739130434782608</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>8.2608695652173907</v>
+        <v>8.695652173913043</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>59.573195793206274</v>
+        <v>60.007978401901923</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.27837941959442186</v>
+        <v>0.28041111402757907</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados en migración
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94:D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,7 +2575,7 @@
         <v>234</v>
       </c>
       <c r="D32" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -3115,7 +3115,7 @@
         <v>269</v>
       </c>
       <c r="D68" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="3"/>
     </row>
@@ -3130,7 +3130,7 @@
         <v>270</v>
       </c>
       <c r="D69" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="3"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4791,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5162,7 +5162,7 @@
         <v>448</v>
       </c>
       <c r="C33" s="3">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6935,7 +6935,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.21739130434782608</v>
+        <v>0.2391304347826087</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>8.695652173913043</v>
+        <v>9.5652173913043477</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>8.25</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>9.9397590361445784E-2</v>
+        <v>0.1030120481927711</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>11.927710843373495</v>
+        <v>12.361445783132531</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>60.007978401901923</v>
+        <v>61.311278559052262</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.28041111402757907</v>
+        <v>0.28650130167781429</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados en componente y carga de archivos project
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94:D94"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2305,7 @@
         <v>216</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3577,7 +3577,7 @@
   <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3716,7 +3716,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="3">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3727,7 +3727,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3738,7 +3738,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3749,7 +3749,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4134,7 +4134,7 @@
         <v>67</v>
       </c>
       <c r="C50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4618,7 +4618,7 @@
         <v>105</v>
       </c>
       <c r="C94" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4791,8 +4791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4887,7 +4887,7 @@
         <v>423</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5162,7 +5162,7 @@
         <v>448</v>
       </c>
       <c r="C33" s="3">
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5206,7 +5206,7 @@
         <v>451</v>
       </c>
       <c r="C37" s="3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -5739,7 +5739,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -6935,7 +6935,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7066,18 +7066,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.26923076923076922</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>5.3846153846153841</v>
+        <v>6.1538461538461542</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>8.5500000000000007</v>
+        <v>8.9</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.1030120481927711</v>
+        <v>0.10722891566265061</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>12.361445783132531</v>
+        <v>12.867469879518072</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>61.311278559052262</v>
+        <v>62.586533424668573</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.28650130167781429</v>
+        <v>0.29246043656387183</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados al proyecto
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
     <sheet name="Daos" sheetId="2" r:id="rId2"/>
-    <sheet name="Vistas" sheetId="3" r:id="rId3"/>
-    <sheet name="FluentValidation" sheetId="5" r:id="rId4"/>
+    <sheet name="FluentValidation" sheetId="5" r:id="rId3"/>
+    <sheet name="Vistas" sheetId="3" r:id="rId4"/>
     <sheet name="Avance" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2305,7 @@
         <v>216</v>
       </c>
       <c r="D14" s="3">
-        <v>0.05</v>
+        <v>0.9</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -2320,7 +2320,7 @@
         <v>217</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -2335,7 +2335,7 @@
         <v>218</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -2575,7 +2575,7 @@
         <v>234</v>
       </c>
       <c r="D32" s="3">
-        <v>0.05</v>
+        <v>0.75</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -3340,7 +3340,7 @@
         <v>284</v>
       </c>
       <c r="D83" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="3"/>
     </row>
@@ -3355,7 +3355,7 @@
         <v>285</v>
       </c>
       <c r="D84" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E84" s="3"/>
     </row>
@@ -3370,7 +3370,7 @@
         <v>286</v>
       </c>
       <c r="D85" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E85" s="3"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,7 +3793,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
         <v>102</v>
       </c>
       <c r="C91" s="1">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>103</v>
       </c>
       <c r="C92" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
         <v>104</v>
       </c>
       <c r="C93" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -4789,16 +4789,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4807,9 +4806,9 @@
         <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4818,10 +4817,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>417</v>
+        <v>318</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4829,10 +4828,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>418</v>
+        <v>319</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4840,10 +4839,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>419</v>
+        <v>320</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4851,10 +4850,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>420</v>
+        <v>321</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4862,10 +4861,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>421</v>
+        <v>317</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4873,10 +4872,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>422</v>
+        <v>322</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4884,10 +4883,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>423</v>
+        <v>323</v>
       </c>
       <c r="C8" s="3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4895,10 +4894,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>424</v>
+        <v>324</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4906,10 +4905,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>425</v>
+        <v>325</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4917,10 +4916,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>426</v>
+        <v>326</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4928,10 +4927,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>427</v>
+        <v>327</v>
       </c>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4939,10 +4938,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>428</v>
+        <v>328</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4950,10 +4949,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>429</v>
+        <v>329</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4961,10 +4960,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>430</v>
+        <v>330</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4972,10 +4971,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>431</v>
+        <v>331</v>
       </c>
       <c r="C16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4983,10 +4982,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>432</v>
+        <v>332</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4994,10 +4993,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>433</v>
+        <v>333</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5005,10 +5004,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>434</v>
+        <v>334</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5016,10 +5015,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>435</v>
+        <v>335</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5027,10 +5026,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>436</v>
+        <v>336</v>
       </c>
       <c r="C21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5038,10 +5037,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>437</v>
+        <v>337</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5049,7 +5048,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>438</v>
+        <v>338</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -5060,7 +5059,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>439</v>
+        <v>339</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -5071,10 +5070,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>440</v>
+        <v>340</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5082,10 +5081,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>441</v>
+        <v>341</v>
       </c>
       <c r="C26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5093,7 +5092,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>442</v>
+        <v>342</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -5104,10 +5103,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>443</v>
+        <v>343</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5115,10 +5114,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>444</v>
+        <v>344</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5126,10 +5125,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>445</v>
+        <v>345</v>
       </c>
       <c r="C30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5137,10 +5136,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>446</v>
+        <v>346</v>
       </c>
       <c r="C31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5148,10 +5147,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>447</v>
+        <v>347</v>
       </c>
       <c r="C32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5159,10 +5158,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>448</v>
+        <v>348</v>
       </c>
       <c r="C33" s="3">
-        <v>0.85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5170,7 +5169,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>449</v>
+        <v>349</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -5181,7 +5180,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>498</v>
+        <v>350</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
@@ -5192,10 +5191,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>450</v>
+        <v>351</v>
       </c>
       <c r="C36" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5203,7 +5202,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>451</v>
+        <v>352</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -5214,7 +5213,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>497</v>
+        <v>353</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -5225,10 +5224,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>452</v>
+        <v>354</v>
       </c>
       <c r="C39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5236,10 +5235,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>453</v>
+        <v>355</v>
       </c>
       <c r="C40" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5247,10 +5246,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>454</v>
+        <v>356</v>
       </c>
       <c r="C41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5258,10 +5257,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>455</v>
+        <v>357</v>
       </c>
       <c r="C42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5269,10 +5268,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="C43" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5280,10 +5279,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>457</v>
+        <v>358</v>
       </c>
       <c r="C44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5291,10 +5290,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>458</v>
+        <v>359</v>
       </c>
       <c r="C45" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5302,10 +5301,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>459</v>
+        <v>360</v>
       </c>
       <c r="C46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5313,10 +5312,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>460</v>
+        <v>361</v>
       </c>
       <c r="C47" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5324,10 +5323,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>478</v>
+        <v>362</v>
       </c>
       <c r="C48" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5335,10 +5334,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>479</v>
+        <v>363</v>
       </c>
       <c r="C49" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5346,10 +5345,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>480</v>
+        <v>364</v>
       </c>
       <c r="C50" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5357,10 +5356,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>481</v>
+        <v>365</v>
       </c>
       <c r="C51" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5368,10 +5367,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>482</v>
+        <v>366</v>
       </c>
       <c r="C52" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5379,10 +5378,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>483</v>
+        <v>367</v>
       </c>
       <c r="C53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5390,10 +5389,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>484</v>
+        <v>368</v>
       </c>
       <c r="C54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5401,10 +5400,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>485</v>
+        <v>369</v>
       </c>
       <c r="C55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5412,10 +5411,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>486</v>
+        <v>370</v>
       </c>
       <c r="C56" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5423,10 +5422,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>487</v>
+        <v>371</v>
       </c>
       <c r="C57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5434,10 +5433,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>488</v>
+        <v>415</v>
       </c>
       <c r="C58" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5445,10 +5444,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>489</v>
+        <v>372</v>
       </c>
       <c r="C59" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5456,10 +5455,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>490</v>
+        <v>373</v>
       </c>
       <c r="C60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5467,10 +5466,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>491</v>
+        <v>374</v>
       </c>
       <c r="C61" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5478,10 +5477,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>492</v>
+        <v>375</v>
       </c>
       <c r="C62" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5489,10 +5488,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>493</v>
+        <v>376</v>
       </c>
       <c r="C63" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5500,10 +5499,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>494</v>
+        <v>377</v>
       </c>
       <c r="C64" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -5511,10 +5510,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>495</v>
+        <v>378</v>
       </c>
       <c r="C65" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -5522,10 +5521,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>496</v>
+        <v>379</v>
       </c>
       <c r="C66" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -5533,10 +5532,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>461</v>
+        <v>380</v>
       </c>
       <c r="C67" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5544,10 +5543,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>462</v>
+        <v>381</v>
       </c>
       <c r="C68" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -5555,10 +5554,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>463</v>
+        <v>382</v>
       </c>
       <c r="C69" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -5566,10 +5565,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>464</v>
+        <v>383</v>
       </c>
       <c r="C70" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -5577,10 +5576,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>465</v>
+        <v>384</v>
       </c>
       <c r="C71" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -5588,10 +5587,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>466</v>
+        <v>385</v>
       </c>
       <c r="C72" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -5599,10 +5598,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>467</v>
+        <v>386</v>
       </c>
       <c r="C73" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -5610,10 +5609,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>468</v>
+        <v>387</v>
       </c>
       <c r="C74" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -5621,10 +5620,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>469</v>
+        <v>388</v>
       </c>
       <c r="C75" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -5632,10 +5631,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>470</v>
+        <v>389</v>
       </c>
       <c r="C76" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5643,10 +5642,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>471</v>
+        <v>390</v>
       </c>
       <c r="C77" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -5654,10 +5653,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>472</v>
+        <v>391</v>
       </c>
       <c r="C78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -5665,10 +5664,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>473</v>
+        <v>392</v>
       </c>
       <c r="C79" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -5676,10 +5675,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>474</v>
+        <v>393</v>
       </c>
       <c r="C80" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -5687,10 +5686,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>475</v>
+        <v>394</v>
       </c>
       <c r="C81" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -5698,10 +5697,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>476</v>
+        <v>395</v>
       </c>
       <c r="C82" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -5709,41 +5708,239 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>477</v>
+        <v>396</v>
       </c>
       <c r="C83" s="3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>397</v>
+      </c>
+      <c r="C84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>398</v>
+      </c>
+      <c r="C85" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+      <c r="A86" s="4">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>399</v>
+      </c>
+      <c r="C86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>400</v>
+      </c>
+      <c r="C87" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>401</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>402</v>
+      </c>
+      <c r="C89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>403</v>
+      </c>
+      <c r="C90" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>404</v>
+      </c>
+      <c r="C91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>405</v>
+      </c>
+      <c r="C92" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>406</v>
+      </c>
+      <c r="C93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>407</v>
+      </c>
+      <c r="C94" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>408</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>409</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>410</v>
+      </c>
+      <c r="C97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>411</v>
+      </c>
+      <c r="C98" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>412</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>413</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>414</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C86">
-        <f>COUNTIFS(C2:C83,100%)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+      <c r="C103">
+        <f>COUNTIFS(C1:C101,100%)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C87">
-        <f>COUNTIFS(C2:C83,"&gt;"&amp; 0%,C2:C83,"&lt;" &amp; 100%)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+      <c r="C104">
+        <f>COUNTIFS(C1:C92,"&gt;"&amp; 0%,C1:C92,"&lt;" &amp; 100%)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C88">
-        <f>COUNTIFS(C2:C83,0%)</f>
-        <v>73</v>
+      <c r="C105">
+        <f>COUNTIFS(C1:C92,0%)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C83">
+  <conditionalFormatting sqref="C2:C101">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5762,15 +5959,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5779,9 +5977,9 @@
         <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5790,10 +5988,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>318</v>
+        <v>417</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5801,10 +5999,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
+        <v>418</v>
       </c>
       <c r="C3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5812,10 +6010,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>419</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5823,10 +6021,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>420</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5834,10 +6032,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>317</v>
+        <v>421</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5845,10 +6043,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>322</v>
+        <v>422</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5856,10 +6054,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>323</v>
+        <v>423</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5867,7 +6065,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>324</v>
+        <v>424</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -5878,7 +6076,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>325</v>
+        <v>425</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -5889,10 +6087,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>326</v>
+        <v>426</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5900,10 +6098,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>327</v>
+        <v>427</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5911,10 +6109,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>328</v>
+        <v>428</v>
       </c>
       <c r="C13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5922,10 +6120,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
+        <v>429</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5933,10 +6131,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>330</v>
+        <v>430</v>
       </c>
       <c r="C15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5944,10 +6142,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>331</v>
+        <v>431</v>
       </c>
       <c r="C16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5955,10 +6153,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5966,10 +6164,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>333</v>
+        <v>433</v>
       </c>
       <c r="C18" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -5977,10 +6175,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>334</v>
+        <v>434</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5988,10 +6186,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>335</v>
+        <v>435</v>
       </c>
       <c r="C20" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5999,10 +6197,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>336</v>
+        <v>436</v>
       </c>
       <c r="C21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6010,10 +6208,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>337</v>
+        <v>437</v>
       </c>
       <c r="C22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6021,7 +6219,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>338</v>
+        <v>438</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -6032,7 +6230,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>339</v>
+        <v>439</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -6043,10 +6241,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>340</v>
+        <v>440</v>
       </c>
       <c r="C25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6054,10 +6252,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>341</v>
+        <v>441</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6065,7 +6263,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>342</v>
+        <v>442</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
@@ -6076,10 +6274,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>343</v>
+        <v>443</v>
       </c>
       <c r="C28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6087,10 +6285,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>344</v>
+        <v>444</v>
       </c>
       <c r="C29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6098,10 +6296,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>345</v>
+        <v>445</v>
       </c>
       <c r="C30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6109,10 +6307,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>346</v>
+        <v>446</v>
       </c>
       <c r="C31" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6120,10 +6318,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>347</v>
+        <v>447</v>
       </c>
       <c r="C32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6131,7 +6329,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="C33" s="3">
         <v>1</v>
@@ -6142,7 +6340,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>349</v>
+        <v>449</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
@@ -6153,7 +6351,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>350</v>
+        <v>498</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
@@ -6164,10 +6362,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>351</v>
+        <v>450</v>
       </c>
       <c r="C36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6175,7 +6373,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>352</v>
+        <v>451</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
@@ -6186,7 +6384,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>353</v>
+        <v>497</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
@@ -6197,10 +6395,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>354</v>
+        <v>452</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6208,10 +6406,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>355</v>
+        <v>453</v>
       </c>
       <c r="C40" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6219,10 +6417,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>356</v>
+        <v>454</v>
       </c>
       <c r="C41" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6230,10 +6428,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>357</v>
+        <v>455</v>
       </c>
       <c r="C42" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6241,10 +6439,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>416</v>
+        <v>456</v>
       </c>
       <c r="C43" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6252,10 +6450,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>358</v>
+        <v>457</v>
       </c>
       <c r="C44" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6263,10 +6461,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>359</v>
+        <v>458</v>
       </c>
       <c r="C45" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -6274,10 +6472,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>360</v>
+        <v>459</v>
       </c>
       <c r="C46" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6285,10 +6483,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>361</v>
+        <v>460</v>
       </c>
       <c r="C47" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6296,10 +6494,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>362</v>
+        <v>478</v>
       </c>
       <c r="C48" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6307,10 +6505,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>363</v>
+        <v>479</v>
       </c>
       <c r="C49" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6318,10 +6516,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>364</v>
+        <v>480</v>
       </c>
       <c r="C50" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6329,10 +6527,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>365</v>
+        <v>481</v>
       </c>
       <c r="C51" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6340,10 +6538,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>366</v>
+        <v>482</v>
       </c>
       <c r="C52" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6351,10 +6549,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>367</v>
+        <v>483</v>
       </c>
       <c r="C53" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6362,10 +6560,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>368</v>
+        <v>484</v>
       </c>
       <c r="C54" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6373,10 +6571,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>369</v>
+        <v>485</v>
       </c>
       <c r="C55" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6384,10 +6582,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>370</v>
+        <v>486</v>
       </c>
       <c r="C56" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6395,10 +6593,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>371</v>
+        <v>487</v>
       </c>
       <c r="C57" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6406,10 +6604,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>415</v>
+        <v>488</v>
       </c>
       <c r="C58" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6417,10 +6615,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>372</v>
+        <v>489</v>
       </c>
       <c r="C59" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6428,10 +6626,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>373</v>
+        <v>490</v>
       </c>
       <c r="C60" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6439,10 +6637,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>374</v>
+        <v>491</v>
       </c>
       <c r="C61" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6450,10 +6648,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>375</v>
+        <v>492</v>
       </c>
       <c r="C62" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6461,10 +6659,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>376</v>
+        <v>493</v>
       </c>
       <c r="C63" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -6472,10 +6670,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>377</v>
+        <v>494</v>
       </c>
       <c r="C64" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -6483,10 +6681,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>378</v>
+        <v>495</v>
       </c>
       <c r="C65" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6494,10 +6692,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>379</v>
+        <v>496</v>
       </c>
       <c r="C66" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6505,10 +6703,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>380</v>
+        <v>461</v>
       </c>
       <c r="C67" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6516,10 +6714,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>381</v>
+        <v>462</v>
       </c>
       <c r="C68" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6527,10 +6725,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>382</v>
+        <v>463</v>
       </c>
       <c r="C69" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6538,10 +6736,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>383</v>
+        <v>464</v>
       </c>
       <c r="C70" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6549,10 +6747,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>384</v>
+        <v>465</v>
       </c>
       <c r="C71" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6560,10 +6758,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>385</v>
+        <v>466</v>
       </c>
       <c r="C72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -6571,10 +6769,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>386</v>
+        <v>467</v>
       </c>
       <c r="C73" s="3">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6582,10 +6780,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>387</v>
+        <v>468</v>
       </c>
       <c r="C74" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6593,10 +6791,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>388</v>
+        <v>469</v>
       </c>
       <c r="C75" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6604,10 +6802,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>389</v>
+        <v>470</v>
       </c>
       <c r="C76" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6615,10 +6813,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>390</v>
+        <v>471</v>
       </c>
       <c r="C77" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6626,10 +6824,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>391</v>
+        <v>472</v>
       </c>
       <c r="C78" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6637,10 +6835,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>392</v>
+        <v>473</v>
       </c>
       <c r="C79" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -6648,10 +6846,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>393</v>
+        <v>474</v>
       </c>
       <c r="C80" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6659,10 +6857,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>394</v>
+        <v>475</v>
       </c>
       <c r="C81" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -6670,10 +6868,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>395</v>
+        <v>476</v>
       </c>
       <c r="C82" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -6681,239 +6879,41 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>396</v>
+        <v>477</v>
       </c>
       <c r="C83" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
-        <v>83</v>
-      </c>
-      <c r="B84" t="s">
-        <v>397</v>
-      </c>
-      <c r="C84" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
-        <v>84</v>
-      </c>
-      <c r="B85" t="s">
-        <v>398</v>
-      </c>
-      <c r="C85" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
-        <v>85</v>
-      </c>
-      <c r="B86" t="s">
-        <v>399</v>
-      </c>
-      <c r="C86" s="3">
-        <v>1</v>
+      <c r="B86" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86">
+        <f>COUNTIFS(C2:C83,100%)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>400</v>
-      </c>
-      <c r="C87" s="3">
-        <v>1</v>
+      <c r="B87" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C87">
+        <f>COUNTIFS(C2:C83,"&gt;"&amp; 0%,C2:C83,"&lt;" &amp; 100%)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>401</v>
-      </c>
-      <c r="C88" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>402</v>
-      </c>
-      <c r="C89" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>403</v>
-      </c>
-      <c r="C90" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
-        <v>404</v>
-      </c>
-      <c r="C91" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
-        <v>405</v>
-      </c>
-      <c r="C92" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
-        <v>92</v>
-      </c>
-      <c r="B93" t="s">
-        <v>406</v>
-      </c>
-      <c r="C93" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
-        <v>93</v>
-      </c>
-      <c r="B94" t="s">
-        <v>407</v>
-      </c>
-      <c r="C94" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>408</v>
-      </c>
-      <c r="C95" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>95</v>
-      </c>
-      <c r="B96" t="s">
-        <v>409</v>
-      </c>
-      <c r="C96" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
-        <v>96</v>
-      </c>
-      <c r="B97" t="s">
-        <v>410</v>
-      </c>
-      <c r="C97" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
-        <v>97</v>
-      </c>
-      <c r="B98" t="s">
-        <v>411</v>
-      </c>
-      <c r="C98" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
-        <v>98</v>
-      </c>
-      <c r="B99" t="s">
-        <v>412</v>
-      </c>
-      <c r="C99" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
-        <v>99</v>
-      </c>
-      <c r="B100" t="s">
-        <v>413</v>
-      </c>
-      <c r="C100" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
-        <v>100</v>
-      </c>
-      <c r="B101" t="s">
-        <v>414</v>
-      </c>
-      <c r="C101" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C103">
-        <f>COUNTIFS(C1:C101,100%)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C104">
-        <f>COUNTIFS(C1:C92,"&gt;"&amp; 0%,C1:C92,"&lt;" &amp; 100%)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C105">
-        <f>COUNTIFS(C1:C92,0%)</f>
-        <v>0</v>
+      <c r="C88">
+        <f>COUNTIFS(C2:C83,0%)</f>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C101">
+  <conditionalFormatting sqref="C2:C83">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -6934,7 +6934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7066,18 +7066,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.30769230769230771</v>
+        <v>0.33653846153846156</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>6.1538461538461542</v>
+        <v>6.7307692307692317</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.2391304347826087</v>
+        <v>0.27173913043478259</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>9.5652173913043477</v>
+        <v>10.869565217391305</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>8.9</v>
+        <v>12</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.10722891566265061</v>
+        <v>0.14457831325301204</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>12.867469879518072</v>
+        <v>17.349397590361445</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>62.586533424668573</v>
+        <v>68.949732038521987</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.29246043656387183</v>
+        <v>0.32219500952580366</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados a subcomponente, componente y pep
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3355,7 +3355,7 @@
         <v>285</v>
       </c>
       <c r="D84" s="3">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E84" s="3"/>
     </row>
@@ -3370,7 +3370,7 @@
         <v>286</v>
       </c>
       <c r="D85" s="3">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E85" s="3"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4574,7 +4574,7 @@
         <v>101</v>
       </c>
       <c r="C90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5961,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74:C75"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6057,7 +6057,7 @@
         <v>423</v>
       </c>
       <c r="C8" s="3">
-        <v>0.95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,7 +6772,7 @@
         <v>467</v>
       </c>
       <c r="C73" s="3">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6783,7 +6783,7 @@
         <v>468</v>
       </c>
       <c r="C74" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -6794,7 +6794,7 @@
         <v>469</v>
       </c>
       <c r="C75" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6900,7 +6900,7 @@
       </c>
       <c r="C87">
         <f>COUNTIFS(C2:C83,"&gt;"&amp; 0%,C2:C83,"&lt;" &amp; 100%)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -7066,18 +7066,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.33653846153846156</v>
+        <v>0.34615384615384615</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>6.7307692307692317</v>
+        <v>6.9230769230769234</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.27173913043478259</v>
+        <v>0.29347826086956524</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>10.869565217391305</v>
+        <v>11.739130434782609</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>12</v>
+        <v>14.5</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.14457831325301204</v>
+        <v>0.1746987951807229</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>17.349397590361445</v>
+        <v>20.963855421686748</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>68.949732038521987</v>
+        <v>73.626062779546274</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.32219500952580366</v>
+        <v>0.34404702233432838</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados producto, producto propiedad, producto tipo, producto controller y otros cambios
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,7 +2305,7 @@
         <v>216</v>
       </c>
       <c r="D14" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -3010,7 +3010,7 @@
         <v>262</v>
       </c>
       <c r="D61" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" s="3"/>
     </row>
@@ -3025,7 +3025,7 @@
         <v>263</v>
       </c>
       <c r="D62" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="3"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,7 +3727,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3815,7 +3815,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="3">
-        <v>0.11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4013,7 +4013,7 @@
         <v>59</v>
       </c>
       <c r="C39" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>64</v>
       </c>
       <c r="C47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4112,7 +4112,7 @@
         <v>65</v>
       </c>
       <c r="C48" s="1">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4123,7 +4123,7 @@
         <v>66</v>
       </c>
       <c r="C49" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4222,7 +4222,7 @@
         <v>72</v>
       </c>
       <c r="C58" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -4244,7 +4244,7 @@
         <v>74</v>
       </c>
       <c r="C60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>76</v>
       </c>
       <c r="C62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -4354,7 +4354,7 @@
         <v>21</v>
       </c>
       <c r="C70" s="1">
-        <v>0.85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4585,7 +4585,7 @@
         <v>102</v>
       </c>
       <c r="C91" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -5961,7 +5961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
@@ -6772,7 +6772,7 @@
         <v>467</v>
       </c>
       <c r="C73" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6900,7 +6900,7 @@
       </c>
       <c r="C87">
         <f>COUNTIFS(C2:C83,"&gt;"&amp; 0%,C2:C83,"&lt;" &amp; 100%)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -7066,18 +7066,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.34615384615384615</v>
+        <v>0.42307692307692307</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>6.9230769230769234</v>
+        <v>8.4615384615384617</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.29347826086956524</v>
+        <v>0.32608695652173914</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>11.739130434782609</v>
+        <v>13.043478260869566</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.1746987951807229</v>
+        <v>0.18674698795180722</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>20.963855421686748</v>
+        <v>22.409638554216865</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>73.626062779546274</v>
+        <v>77.914655276624899</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.34404702233432838</v>
+        <v>0.36408717418983599</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Se suben cambios de subproducto y cambios de correcciones en otros componentes dle sistema
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,7 +3040,7 @@
         <v>264</v>
       </c>
       <c r="D63" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" s="3"/>
     </row>
@@ -3385,7 +3385,7 @@
         <v>287</v>
       </c>
       <c r="D86" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E86" s="3"/>
     </row>
@@ -3400,7 +3400,7 @@
         <v>288</v>
       </c>
       <c r="D87" s="3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E87" s="3"/>
     </row>
@@ -3415,7 +3415,7 @@
         <v>289</v>
       </c>
       <c r="D88" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E88" s="3"/>
     </row>
@@ -3514,7 +3514,7 @@
       <c r="C97" s="4"/>
       <c r="D97">
         <f>COUNTIFS(D3:D94,100%)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4233,7 +4233,7 @@
         <v>73</v>
       </c>
       <c r="C59" s="1">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4629,7 +4629,7 @@
         <v>106</v>
       </c>
       <c r="C95" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -4651,7 +4651,7 @@
         <v>108</v>
       </c>
       <c r="C97" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -4662,7 +4662,7 @@
         <v>109</v>
       </c>
       <c r="C98" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -4673,7 +4673,7 @@
         <v>110</v>
       </c>
       <c r="C99" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C108">
         <f>COUNTIFS(C2:C105,100%)</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="C109">
         <f>COUNTIFS(C2:C105,"&gt;"&amp; 0%,C2:C105,"&lt;" &amp; 100%)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="C110">
         <f>COUNTIFS(C2:C105,0%)</f>
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -5961,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6398,7 +6398,7 @@
         <v>452</v>
       </c>
       <c r="C39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6409,7 +6409,7 @@
         <v>453</v>
       </c>
       <c r="C40" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6420,7 +6420,7 @@
         <v>454</v>
       </c>
       <c r="C41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6805,7 +6805,7 @@
         <v>470</v>
       </c>
       <c r="C76" s="3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -6816,7 +6816,7 @@
         <v>471</v>
       </c>
       <c r="C77" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -6827,7 +6827,7 @@
         <v>472</v>
       </c>
       <c r="C78" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="C86">
         <f>COUNTIFS(C2:C83,100%)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -6900,7 +6900,7 @@
       </c>
       <c r="C87">
         <f>COUNTIFS(C2:C83,"&gt;"&amp; 0%,C2:C83,"&lt;" &amp; 100%)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="C88">
         <f>COUNTIFS(C2:C83,0%)</f>
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -7066,18 +7066,18 @@
       </c>
       <c r="D8" s="9">
         <f>Daos!C108</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="1"/>
-        <v>0.42307692307692307</v>
+        <v>0.44230769230769229</v>
       </c>
       <c r="F8" s="9">
         <v>20</v>
       </c>
       <c r="G8" s="12">
         <f t="shared" si="0"/>
-        <v>8.4615384615384617</v>
+        <v>8.8461538461538467</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7090,18 +7090,18 @@
       </c>
       <c r="D9" s="9">
         <f>Controllers!D97</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="1"/>
-        <v>0.32608695652173914</v>
+        <v>0.33695652173913043</v>
       </c>
       <c r="F9" s="9">
         <v>40</v>
       </c>
       <c r="G9" s="12">
         <f t="shared" si="0"/>
-        <v>13.043478260869566</v>
+        <v>13.478260869565217</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7134,18 +7134,18 @@
         <v>83</v>
       </c>
       <c r="D11" s="9">
-        <v>15.5</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.18674698795180722</v>
+        <v>0.24578313253012046</v>
       </c>
       <c r="F11" s="9">
         <v>120</v>
       </c>
       <c r="G11" s="12">
         <f t="shared" si="0"/>
-        <v>22.409638554216865</v>
+        <v>29.493975903614455</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -7185,7 +7185,7 @@
       </c>
       <c r="G13" s="12">
         <f>SUM(G4:G12)</f>
-        <v>77.914655276624899</v>
+        <v>85.818390619333513</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="33.75" x14ac:dyDescent="0.5">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="C16" s="15">
         <f>G13/F13</f>
-        <v>0.36408717418983599</v>
+        <v>0.40102051691277341</v>
       </c>
       <c r="D16" s="15"/>
     </row>

</xml_diff>

<commit_message>
Cambios realizados a actividad
</commit_message>
<xml_diff>
--- a/Avances/Avance Migracion Sipro.xlsx
+++ b/Avances/Avance Migracion Sipro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2140,7 @@
         <v>205</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -3524,7 +3524,7 @@
       <c r="C98" s="4"/>
       <c r="D98">
         <f>COUNTIFS(D3:D94,"&gt;"&amp; 0%,D3:D94,"&lt;" &amp; 100%)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
       <c r="C99" s="4"/>
       <c r="D99">
         <f>COUNTIFS(D3:D94,0%)</f>
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78:C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5961,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77:C78"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6934,8 +6934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>